<commit_message>
Increased version to 1.5.1
</commit_message>
<xml_diff>
--- a/DCSortment/bin/Debug/double.xlsx
+++ b/DCSortment/bin/Debug/double.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>House</t>
   </si>
@@ -24,19 +24,28 @@
     <t>Ratings</t>
   </si>
   <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>Bravo</t>
-  </si>
-  <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t>Echo</t>
-  </si>
-  <si>
-    <t>Delta</t>
+    <t>dne</t>
+  </si>
+  <si>
+    <t>GREENKEY</t>
+  </si>
+  <si>
+    <t>PURPLEKEY</t>
+  </si>
+  <si>
+    <t>REDKEY</t>
+  </si>
+  <si>
+    <t>ALPHAKEY</t>
+  </si>
+  <si>
+    <t>ACETAKEY</t>
+  </si>
+  <si>
+    <t>BETAKEY</t>
+  </si>
+  <si>
+    <t>CHARLIEKEY</t>
   </si>
 </sst>
 </file>
@@ -378,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,35 +410,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
+        <v>98.1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,21 +446,43 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
+        <v>98.55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
+      </c>
+      <c r="B7">
+        <v>98.6</v>
+      </c>
+      <c r="C7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version increased to 1.5.3
</commit_message>
<xml_diff>
--- a/DCSortment/bin/Debug/double.xlsx
+++ b/DCSortment/bin/Debug/double.xlsx
@@ -390,7 +390,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,11 +423,11 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>98.1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>